<commit_message>
adding PSM QC and one hit wonder analysis
</commit_message>
<xml_diff>
--- a/shared/Quick summary methods.xlsx
+++ b/shared/Quick summary methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/mawe2_cam_ac_uk/Documents/MRC/Analysis/hyperplexed/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{41D9DFD6-AF39-2747-981D-A2405BBC7DD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B3558321-B3B6-B342-A8F5-F2568CBC28B0}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{41D9DFD6-AF39-2747-981D-A2405BBC7DD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E785A1F7-D079-8348-9DCF-FF28536950DE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{98EA5DBC-0B00-5942-A6B1-5895EAB89A05}"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="22320" windowHeight="13560" xr2:uid="{98EA5DBC-0B00-5942-A6B1-5895EAB89A05}"/>
   </bookViews>
   <sheets>
     <sheet name="different methods used" sheetId="1" r:id="rId1"/>
@@ -494,7 +494,7 @@
       <pane xSplit="2" ySplit="17" topLeftCell="K18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" sqref="A1:B1048576"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>